<commit_message>
Update turkey corona data 25.03.2020.xlsx
</commit_message>
<xml_diff>
--- a/turkey corona data 25.03.2020.xlsx
+++ b/turkey corona data 25.03.2020.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mert Can\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mert Can\Documents\GitHub\coronaData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8FB060B-8E3D-4918-82C4-CEE77AD32996}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB4C546D-15FC-41CC-87FA-6C69EAA23803}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{28E687B1-0B9C-4FA1-ACD1-56D21E9B63E9}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{28E687B1-0B9C-4FA1-ACD1-56D21E9B63E9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Day</t>
   </si>
@@ -37,6 +37,9 @@
   </si>
   <si>
     <t>Recovered</t>
+  </si>
+  <si>
+    <t>Test Number</t>
   </si>
 </sst>
 </file>
@@ -1615,20 +1618,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAC64E10-8C86-417F-8B6B-95226FC28549}">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="4" width="14.5703125" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="1"/>
+    <col min="2" max="5" width="14.28515625" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1641,8 +1644,11 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1656,7 +1662,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1670,7 +1676,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1684,7 +1690,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1698,7 +1704,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1712,7 +1718,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1726,7 +1732,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1740,7 +1746,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1754,7 +1760,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1768,7 +1774,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1782,7 +1788,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -1796,7 +1802,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -1810,7 +1816,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -1824,7 +1830,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -1838,7 +1844,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -1851,8 +1857,11 @@
       <c r="D16" s="1">
         <v>26</v>
       </c>
+      <c r="E16" s="1">
+        <v>5035</v>
+      </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -1864,6 +1873,9 @@
       </c>
       <c r="D17" s="1">
         <v>26</v>
+      </c>
+      <c r="E17" s="1">
+        <v>7286</v>
       </c>
     </row>
   </sheetData>

</xml_diff>